<commit_message>
Fixed PI total funding bug
Accidentally counted funding per connection
</commit_message>
<xml_diff>
--- a/datasheets/ALL Funded ARCHES Projects.xlsx
+++ b/datasheets/ALL Funded ARCHES Projects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinho\Documents\UIUC\OSF Academic Collaborations\Github\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC87F85-D856-44DB-A38C-14CF130E04BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0F48F1-0642-4C04-8CB5-6CFCD1AE998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="1153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2986" uniqueCount="1152">
   <si>
     <t>Year</t>
   </si>
@@ -1946,9 +1946,6 @@
     <t>P012</t>
   </si>
   <si>
-    <t>Multimodal Image-Guided Surgery and 3d Visualiztion System</t>
-  </si>
-  <si>
     <t>https://app.box.com/file/59157081573</t>
   </si>
   <si>
@@ -3311,9 +3308,6 @@
     <t>P351</t>
   </si>
   <si>
-    <t>Brad Suton</t>
-  </si>
-  <si>
     <t>P352</t>
   </si>
   <si>
@@ -3528,6 +3522,9 @@
   </si>
   <si>
     <t>54 57 8</t>
+  </si>
+  <si>
+    <t>Multimodal Image-Guided Surgery and 3d Visualization System</t>
   </si>
 </sst>
 </file>
@@ -5245,8 +5242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K127" sqref="K127"/>
+    <sheetView tabSelected="1" topLeftCell="F84" zoomScale="86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -5651,7 +5648,7 @@
         <v>66</v>
       </c>
       <c r="F7" s="102" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G7" s="101" t="s">
         <v>67</v>
@@ -7398,7 +7395,7 @@
         <v>234</v>
       </c>
       <c r="Q35" s="96" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="R35" s="96" t="s">
         <v>235</v>
@@ -7523,7 +7520,7 @@
         <v>245</v>
       </c>
       <c r="F37" s="102" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G37" s="101" t="s">
         <v>246</v>
@@ -8238,7 +8235,7 @@
         <v>314</v>
       </c>
       <c r="L47" s="96" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="M47" s="96" t="s">
         <v>104</v>
@@ -8845,7 +8842,7 @@
         <v>261</v>
       </c>
       <c r="J56" s="96" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="K56" s="96" t="s">
         <v>374</v>
@@ -8904,7 +8901,7 @@
         <v>380</v>
       </c>
       <c r="F57" s="96" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G57" s="105" t="s">
         <v>381</v>
@@ -9122,7 +9119,7 @@
         <v>407</v>
       </c>
       <c r="J60" s="96" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="K60" s="96" t="s">
         <v>408</v>
@@ -9517,7 +9514,7 @@
         <v>555</v>
       </c>
       <c r="J66" s="96" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="K66" s="96" t="s">
         <v>382</v>
@@ -9706,7 +9703,7 @@
         <v>458</v>
       </c>
       <c r="E69" s="102" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F69" s="96" t="s">
         <v>331</v>
@@ -9843,7 +9840,7 @@
         <v>470</v>
       </c>
       <c r="F71" s="102" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="G71" s="105" t="s">
         <v>471</v>
@@ -10205,7 +10202,7 @@
         <v>206</v>
       </c>
       <c r="F76" s="96" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G76" s="105" t="s">
         <v>507</v>
@@ -10429,7 +10426,7 @@
         <v>210</v>
       </c>
       <c r="L79" s="96" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="M79" s="96" t="s">
         <v>509</v>
@@ -11085,7 +11082,7 @@
         <v>35000</v>
       </c>
       <c r="I89" s="111" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="J89" s="111" t="s">
         <v>592</v>
@@ -11334,7 +11331,7 @@
         <v>617</v>
       </c>
       <c r="E93" s="111" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="F93" s="111" t="s">
         <v>426</v>
@@ -11399,14 +11396,14 @@
       </c>
       <c r="F94" s="97"/>
       <c r="G94" s="120" t="s">
-        <v>625</v>
+        <v>1151</v>
       </c>
       <c r="H94" s="124">
         <v>49941</v>
       </c>
       <c r="T94" s="94"/>
       <c r="AC94" s="105" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="95" spans="1:29">
@@ -11416,21 +11413,21 @@
       <c r="B95" s="99"/>
       <c r="C95" s="120"/>
       <c r="D95" s="121" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E95" s="97" t="s">
         <v>78</v>
       </c>
       <c r="F95" s="97"/>
       <c r="G95" s="120" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="H95" s="124">
         <v>48581</v>
       </c>
       <c r="T95" s="94"/>
       <c r="AC95" s="105" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="96" spans="1:29" ht="14.4">
@@ -11441,11 +11438,11 @@
       <c r="C96" s="120"/>
       <c r="D96" s="121"/>
       <c r="E96" s="97" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F96" s="97"/>
       <c r="G96" s="120" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="H96" s="124">
         <v>49362</v>
@@ -11486,7 +11483,7 @@
         <v>29</v>
       </c>
       <c r="D97" s="121" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E97" s="126" t="s">
         <v>570</v>
@@ -11495,7 +11492,7 @@
         <v>347</v>
       </c>
       <c r="G97" s="127" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="H97" s="124">
         <v>75652</v>
@@ -11536,7 +11533,7 @@
         <v>44943</v>
       </c>
       <c r="AB97" s="156" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="98" spans="1:28" ht="14.4">
@@ -11548,7 +11545,7 @@
         <v>29</v>
       </c>
       <c r="D98" s="121" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E98" s="126" t="s">
         <v>96</v>
@@ -11557,7 +11554,7 @@
         <v>439</v>
       </c>
       <c r="G98" s="127" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H98" s="124">
         <v>75000</v>
@@ -11600,7 +11597,7 @@
         <v>44943</v>
       </c>
       <c r="AB98" s="156" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="99" spans="1:28" ht="14.4">
@@ -11612,22 +11609,22 @@
         <v>29</v>
       </c>
       <c r="D99" s="121" t="s">
+        <v>635</v>
+      </c>
+      <c r="E99" s="126" t="s">
         <v>636</v>
       </c>
-      <c r="E99" s="126" t="s">
+      <c r="F99" s="145" t="s">
+        <v>638</v>
+      </c>
+      <c r="G99" s="127" t="s">
         <v>637</v>
-      </c>
-      <c r="F99" s="145" t="s">
-        <v>639</v>
-      </c>
-      <c r="G99" s="127" t="s">
-        <v>638</v>
       </c>
       <c r="H99" s="124">
         <v>38921</v>
       </c>
       <c r="I99" s="153" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J99" s="153"/>
       <c r="K99" s="153"/>
@@ -11664,7 +11661,7 @@
         <v>44943</v>
       </c>
       <c r="AB99" s="156" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="100" spans="1:28" ht="14.4">
@@ -11676,25 +11673,25 @@
         <v>29</v>
       </c>
       <c r="D100" s="121" t="s">
+        <v>640</v>
+      </c>
+      <c r="E100" s="126" t="s">
         <v>641</v>
       </c>
-      <c r="E100" s="126" t="s">
+      <c r="F100" s="139" t="s">
+        <v>643</v>
+      </c>
+      <c r="G100" s="128" t="s">
         <v>642</v>
-      </c>
-      <c r="F100" s="139" t="s">
-        <v>644</v>
-      </c>
-      <c r="G100" s="128" t="s">
-        <v>643</v>
       </c>
       <c r="H100" s="124">
         <v>74892</v>
       </c>
       <c r="I100" s="149" t="s">
+        <v>644</v>
+      </c>
+      <c r="J100" s="153" t="s">
         <v>645</v>
-      </c>
-      <c r="J100" s="153" t="s">
-        <v>646</v>
       </c>
       <c r="K100" s="153"/>
       <c r="L100" s="153"/>
@@ -11730,7 +11727,7 @@
         <v>44943</v>
       </c>
       <c r="AB100" s="156" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="14.4">
@@ -11742,7 +11739,7 @@
         <v>29</v>
       </c>
       <c r="D101" s="121" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E101" s="126" t="s">
         <v>198</v>
@@ -11751,7 +11748,7 @@
         <v>372</v>
       </c>
       <c r="G101" s="127" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H101" s="124">
         <v>149779.872</v>
@@ -11794,7 +11791,7 @@
         <v>44943</v>
       </c>
       <c r="AB101" s="156" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="102" spans="1:28" ht="14.4">
@@ -11806,16 +11803,16 @@
         <v>29</v>
       </c>
       <c r="D102" s="121" t="s">
+        <v>648</v>
+      </c>
+      <c r="E102" s="126" t="s">
         <v>649</v>
-      </c>
-      <c r="E102" s="126" t="s">
-        <v>650</v>
       </c>
       <c r="F102" s="140" t="s">
         <v>372</v>
       </c>
       <c r="G102" s="127" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="H102" s="124">
         <v>75000.000000000015</v>
@@ -11860,7 +11857,7 @@
         <v>44943</v>
       </c>
       <c r="AB102" s="156" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="14.4">
@@ -11872,22 +11869,22 @@
         <v>29</v>
       </c>
       <c r="D103" s="121" t="s">
+        <v>651</v>
+      </c>
+      <c r="E103" s="126" t="s">
         <v>652</v>
-      </c>
-      <c r="E103" s="126" t="s">
-        <v>653</v>
       </c>
       <c r="F103" s="145" t="s">
         <v>524</v>
       </c>
       <c r="G103" s="127" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H103" s="124">
         <v>74802</v>
       </c>
       <c r="I103" s="153" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="J103" s="153" t="s">
         <v>522</v>
@@ -11926,7 +11923,7 @@
         <v>44943</v>
       </c>
       <c r="AB103" s="156" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="104" spans="1:28" ht="14.4">
@@ -11938,16 +11935,16 @@
         <v>29</v>
       </c>
       <c r="D104" s="121" t="s">
+        <v>655</v>
+      </c>
+      <c r="E104" s="126" t="s">
         <v>656</v>
       </c>
-      <c r="E104" s="126" t="s">
+      <c r="F104" s="139" t="s">
+        <v>1087</v>
+      </c>
+      <c r="G104" s="127" t="s">
         <v>657</v>
-      </c>
-      <c r="F104" s="139" t="s">
-        <v>1089</v>
-      </c>
-      <c r="G104" s="127" t="s">
-        <v>658</v>
       </c>
       <c r="H104" s="124">
         <v>74995.78</v>
@@ -11956,7 +11953,7 @@
         <v>589</v>
       </c>
       <c r="J104" s="153" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="K104" s="153" t="s">
         <v>577</v>
@@ -11994,7 +11991,7 @@
         <v>44943</v>
       </c>
       <c r="AB104" s="156" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="14.4">
@@ -12006,7 +12003,7 @@
         <v>29</v>
       </c>
       <c r="D105" s="121" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E105" s="126" t="s">
         <v>355</v>
@@ -12015,7 +12012,7 @@
         <v>352</v>
       </c>
       <c r="G105" s="127" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H105" s="124">
         <v>47234.8</v>
@@ -12058,7 +12055,7 @@
         <v>44943</v>
       </c>
       <c r="AB105" s="156" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="106" spans="1:28" ht="14.4">
@@ -12070,16 +12067,16 @@
         <v>29</v>
       </c>
       <c r="D106" s="121" t="s">
+        <v>661</v>
+      </c>
+      <c r="E106" s="126" t="s">
         <v>662</v>
       </c>
-      <c r="E106" s="126" t="s">
+      <c r="F106" s="139" t="s">
+        <v>664</v>
+      </c>
+      <c r="G106" s="127" t="s">
         <v>663</v>
-      </c>
-      <c r="F106" s="139" t="s">
-        <v>665</v>
-      </c>
-      <c r="G106" s="127" t="s">
-        <v>664</v>
       </c>
       <c r="H106" s="124">
         <v>52666</v>
@@ -12088,31 +12085,31 @@
         <v>491</v>
       </c>
       <c r="J106" s="153" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="K106" s="153" t="s">
+        <v>665</v>
+      </c>
+      <c r="L106" s="153" t="s">
         <v>666</v>
       </c>
-      <c r="L106" s="153" t="s">
+      <c r="M106" s="153" t="s">
         <v>667</v>
       </c>
-      <c r="M106" s="153" t="s">
+      <c r="N106" s="153" t="s">
         <v>668</v>
       </c>
-      <c r="N106" s="153" t="s">
+      <c r="O106" s="153" t="s">
         <v>669</v>
       </c>
-      <c r="O106" s="153" t="s">
+      <c r="P106" s="153" t="s">
         <v>670</v>
-      </c>
-      <c r="P106" s="153" t="s">
-        <v>671</v>
       </c>
       <c r="Q106" s="153" t="s">
         <v>78</v>
       </c>
       <c r="R106" s="153" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="S106" s="145"/>
       <c r="T106" s="155" t="s">
@@ -12140,7 +12137,7 @@
         <v>44943</v>
       </c>
       <c r="AB106" s="156" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="107" spans="1:28" ht="14.4">
@@ -12152,7 +12149,7 @@
         <v>29</v>
       </c>
       <c r="D107" s="121" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E107" s="126" t="s">
         <v>61</v>
@@ -12161,7 +12158,7 @@
         <v>78</v>
       </c>
       <c r="G107" s="127" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H107" s="124">
         <v>74879</v>
@@ -12170,7 +12167,7 @@
         <v>482</v>
       </c>
       <c r="J107" s="153" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K107" s="153"/>
       <c r="L107" s="153"/>
@@ -12206,7 +12203,7 @@
         <v>44943</v>
       </c>
       <c r="AB107" s="156" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="108" spans="1:28" ht="14.4">
@@ -12218,7 +12215,7 @@
         <v>29</v>
       </c>
       <c r="D108" s="121" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E108" s="126" t="s">
         <v>248</v>
@@ -12227,7 +12224,7 @@
         <v>347</v>
       </c>
       <c r="G108" s="127" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="H108" s="124">
         <v>55693</v>
@@ -12268,7 +12265,7 @@
         <v>44943</v>
       </c>
       <c r="AB108" s="156" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="109" spans="1:28" ht="14.4">
@@ -12280,16 +12277,16 @@
         <v>29</v>
       </c>
       <c r="D109" s="121" t="s">
+        <v>677</v>
+      </c>
+      <c r="E109" s="126" t="s">
         <v>678</v>
       </c>
-      <c r="E109" s="126" t="s">
+      <c r="F109" s="145" t="s">
+        <v>680</v>
+      </c>
+      <c r="G109" s="127" t="s">
         <v>679</v>
-      </c>
-      <c r="F109" s="145" t="s">
-        <v>681</v>
-      </c>
-      <c r="G109" s="127" t="s">
-        <v>680</v>
       </c>
       <c r="H109" s="124">
         <v>74340.08</v>
@@ -12298,10 +12295,10 @@
         <v>443</v>
       </c>
       <c r="J109" s="153" t="s">
+        <v>681</v>
+      </c>
+      <c r="K109" s="153" t="s">
         <v>682</v>
-      </c>
-      <c r="K109" s="153" t="s">
-        <v>683</v>
       </c>
       <c r="L109" s="153"/>
       <c r="M109" s="153"/>
@@ -12336,7 +12333,7 @@
         <v>44943</v>
       </c>
       <c r="AB109" s="156" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="110" spans="1:28" ht="14.4">
@@ -12348,22 +12345,22 @@
         <v>29</v>
       </c>
       <c r="D110" s="121" t="s">
+        <v>683</v>
+      </c>
+      <c r="E110" s="126" t="s">
         <v>684</v>
       </c>
-      <c r="E110" s="126" t="s">
+      <c r="F110" s="141" t="s">
+        <v>686</v>
+      </c>
+      <c r="G110" s="127" t="s">
         <v>685</v>
-      </c>
-      <c r="F110" s="141" t="s">
-        <v>687</v>
-      </c>
-      <c r="G110" s="127" t="s">
-        <v>686</v>
       </c>
       <c r="H110" s="124">
         <v>75000</v>
       </c>
       <c r="I110" s="151" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J110" s="153" t="s">
         <v>347</v>
@@ -12402,7 +12399,7 @@
         <v>44943</v>
       </c>
       <c r="AB110" s="156" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="111" spans="1:28" ht="14.4">
@@ -12414,22 +12411,22 @@
         <v>29</v>
       </c>
       <c r="D111" s="121" t="s">
+        <v>688</v>
+      </c>
+      <c r="E111" s="126" t="s">
+        <v>684</v>
+      </c>
+      <c r="F111" s="145" t="s">
+        <v>686</v>
+      </c>
+      <c r="G111" s="127" t="s">
         <v>689</v>
-      </c>
-      <c r="E111" s="126" t="s">
-        <v>685</v>
-      </c>
-      <c r="F111" s="145" t="s">
-        <v>687</v>
-      </c>
-      <c r="G111" s="127" t="s">
-        <v>690</v>
       </c>
       <c r="H111" s="124">
         <v>75000</v>
       </c>
       <c r="I111" s="153" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="J111" s="153" t="s">
         <v>347</v>
@@ -12468,7 +12465,7 @@
         <v>44943</v>
       </c>
       <c r="AB111" s="156" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="14.4">
@@ -12480,22 +12477,22 @@
         <v>29</v>
       </c>
       <c r="D112" s="121" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E112" s="126" t="s">
         <v>185</v>
       </c>
       <c r="F112" s="140" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G112" s="127" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="H112" s="124">
         <v>78810</v>
       </c>
       <c r="I112" s="148" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="J112" s="153"/>
       <c r="K112" s="153"/>
@@ -12532,7 +12529,7 @@
         <v>44943</v>
       </c>
       <c r="AB112" s="156" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="113" spans="1:29" ht="14.4">
@@ -12544,16 +12541,16 @@
         <v>29</v>
       </c>
       <c r="D113" s="121" t="s">
+        <v>695</v>
+      </c>
+      <c r="E113" s="126" t="s">
         <v>696</v>
       </c>
-      <c r="E113" s="126" t="s">
+      <c r="F113" s="145" t="s">
+        <v>698</v>
+      </c>
+      <c r="G113" s="127" t="s">
         <v>697</v>
-      </c>
-      <c r="F113" s="145" t="s">
-        <v>699</v>
-      </c>
-      <c r="G113" s="127" t="s">
-        <v>698</v>
       </c>
       <c r="H113" s="124">
         <v>66278</v>
@@ -12594,7 +12591,7 @@
         <v>44943</v>
       </c>
       <c r="AB113" s="156" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="AC113" s="154"/>
     </row>
@@ -12607,7 +12604,7 @@
         <v>29</v>
       </c>
       <c r="D114" s="121" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E114" s="126" t="s">
         <v>555</v>
@@ -12616,7 +12613,7 @@
         <v>103</v>
       </c>
       <c r="G114" s="127" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="H114" s="124">
         <v>71395</v>
@@ -12625,7 +12622,7 @@
         <v>614</v>
       </c>
       <c r="J114" s="153" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K114" s="153"/>
       <c r="L114" s="153"/>
@@ -12661,7 +12658,7 @@
         <v>44943</v>
       </c>
       <c r="AB114" s="156" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="AC114" s="154"/>
     </row>
@@ -12674,7 +12671,7 @@
         <v>29</v>
       </c>
       <c r="D115" s="121" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E115" s="126" t="s">
         <v>555</v>
@@ -12683,16 +12680,16 @@
         <v>148</v>
       </c>
       <c r="G115" s="128" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H115" s="124">
         <v>71709</v>
       </c>
       <c r="I115" s="153" t="s">
+        <v>703</v>
+      </c>
+      <c r="J115" s="153" t="s">
         <v>704</v>
-      </c>
-      <c r="J115" s="153" t="s">
-        <v>705</v>
       </c>
       <c r="K115" s="153"/>
       <c r="L115" s="153"/>
@@ -12728,7 +12725,7 @@
         <v>44943</v>
       </c>
       <c r="AB115" s="156" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="AC115" s="154"/>
     </row>
@@ -12741,16 +12738,16 @@
         <v>29</v>
       </c>
       <c r="D116" s="121" t="s">
+        <v>705</v>
+      </c>
+      <c r="E116" s="126" t="s">
         <v>706</v>
       </c>
-      <c r="E116" s="126" t="s">
+      <c r="F116" s="130" t="s">
+        <v>1068</v>
+      </c>
+      <c r="G116" s="127" t="s">
         <v>707</v>
-      </c>
-      <c r="F116" s="130" t="s">
-        <v>1069</v>
-      </c>
-      <c r="G116" s="127" t="s">
-        <v>708</v>
       </c>
       <c r="H116" s="124">
         <v>74973.600000000006</v>
@@ -12765,7 +12762,7 @@
         <v>568</v>
       </c>
       <c r="L116" s="153" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="M116" s="153"/>
       <c r="N116" s="153"/>
@@ -12799,7 +12796,7 @@
         <v>44943</v>
       </c>
       <c r="AB116" s="156" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="AC116" s="154"/>
     </row>
@@ -12812,16 +12809,16 @@
         <v>76</v>
       </c>
       <c r="D117" s="134" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E117" s="137" t="s">
+        <v>680</v>
+      </c>
+      <c r="F117" s="131" t="s">
         <v>1070</v>
       </c>
-      <c r="E117" s="137" t="s">
-        <v>681</v>
-      </c>
-      <c r="F117" s="131" t="s">
-        <v>1071</v>
-      </c>
       <c r="G117" s="144" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="H117" s="143">
         <v>74872</v>
@@ -12830,7 +12827,7 @@
         <v>443</v>
       </c>
       <c r="J117" s="152" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="K117" s="152"/>
       <c r="L117" s="152"/>
@@ -12864,7 +12861,7 @@
       </c>
       <c r="AA117" s="157"/>
       <c r="AB117" s="156" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="AC117" s="154"/>
     </row>
@@ -12877,7 +12874,7 @@
         <v>76</v>
       </c>
       <c r="D118" s="136" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E118" s="131" t="s">
         <v>355</v>
@@ -12886,13 +12883,13 @@
         <v>352</v>
       </c>
       <c r="G118" s="142" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="H118" s="143">
         <v>75000</v>
       </c>
       <c r="I118" s="147" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="J118" s="147"/>
       <c r="K118" s="147"/>
@@ -12927,7 +12924,7 @@
       </c>
       <c r="AA118" s="158"/>
       <c r="AB118" s="158" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="AC118" s="158"/>
     </row>
@@ -12940,31 +12937,31 @@
         <v>76</v>
       </c>
       <c r="D119" s="136" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E119" s="131" t="s">
         <v>1073</v>
       </c>
-      <c r="E119" s="131" t="s">
+      <c r="F119" s="137" t="s">
         <v>1074</v>
       </c>
-      <c r="F119" s="137" t="s">
-        <v>1075</v>
-      </c>
       <c r="G119" s="142" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="H119" s="143">
         <v>67712</v>
       </c>
       <c r="I119" s="147" t="s">
+        <v>1102</v>
+      </c>
+      <c r="J119" s="147" t="s">
+        <v>1103</v>
+      </c>
+      <c r="K119" s="147" t="s">
         <v>1104</v>
       </c>
-      <c r="J119" s="147" t="s">
+      <c r="L119" s="147" t="s">
         <v>1105</v>
-      </c>
-      <c r="K119" s="147" t="s">
-        <v>1106</v>
-      </c>
-      <c r="L119" s="147" t="s">
-        <v>1107</v>
       </c>
       <c r="M119" s="147"/>
       <c r="N119" s="147"/>
@@ -12996,7 +12993,7 @@
       </c>
       <c r="AA119" s="158"/>
       <c r="AB119" s="158" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="AC119" s="158"/>
     </row>
@@ -13009,37 +13006,37 @@
         <v>76</v>
       </c>
       <c r="D120" s="136" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E120" s="131" t="s">
         <v>1076</v>
       </c>
-      <c r="E120" s="131" t="s">
-        <v>1077</v>
-      </c>
       <c r="F120" s="137" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="G120" s="142" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="H120" s="143">
         <v>75000</v>
       </c>
       <c r="I120" s="147" t="s">
+        <v>1106</v>
+      </c>
+      <c r="J120" s="147" t="s">
+        <v>1107</v>
+      </c>
+      <c r="K120" s="147" t="s">
+        <v>1027</v>
+      </c>
+      <c r="L120" s="147" t="s">
         <v>1108</v>
       </c>
-      <c r="J120" s="147" t="s">
+      <c r="M120" s="147" t="s">
         <v>1109</v>
       </c>
-      <c r="K120" s="147" t="s">
-        <v>1028</v>
-      </c>
-      <c r="L120" s="147" t="s">
+      <c r="N120" s="147" t="s">
         <v>1110</v>
-      </c>
-      <c r="M120" s="147" t="s">
-        <v>1111</v>
-      </c>
-      <c r="N120" s="147" t="s">
-        <v>1112</v>
       </c>
       <c r="O120" s="147"/>
       <c r="P120" s="147"/>
@@ -13069,7 +13066,7 @@
       </c>
       <c r="AA120" s="158"/>
       <c r="AB120" s="158" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="AC120" s="158"/>
     </row>
@@ -13082,22 +13079,22 @@
         <v>76</v>
       </c>
       <c r="D121" s="136" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E121" s="131" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="F121" s="137" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="G121" s="142" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="H121" s="143">
         <v>74697</v>
       </c>
       <c r="I121" s="147" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="J121" s="147" t="s">
         <v>482</v>
@@ -13134,7 +13131,7 @@
       </c>
       <c r="AA121" s="158"/>
       <c r="AB121" s="158" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="AC121" s="158"/>
     </row>
@@ -13147,16 +13144,16 @@
         <v>76</v>
       </c>
       <c r="D122" s="136" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E122" s="131" t="s">
         <v>61</v>
       </c>
       <c r="F122" s="137" t="s">
-        <v>1080</v>
+        <v>78</v>
       </c>
       <c r="G122" s="142" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="H122" s="143">
         <v>29162</v>
@@ -13195,7 +13192,7 @@
       </c>
       <c r="AA122" s="158"/>
       <c r="AB122" s="158" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="AC122" s="158"/>
     </row>
@@ -13208,7 +13205,7 @@
         <v>76</v>
       </c>
       <c r="D123" s="136" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="E123" s="131" t="s">
         <v>574</v>
@@ -13217,22 +13214,22 @@
         <v>172</v>
       </c>
       <c r="G123" s="142" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="H123" s="143">
         <v>75000</v>
       </c>
       <c r="I123" s="147" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="J123" s="147" t="s">
         <v>578</v>
       </c>
       <c r="K123" s="147" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="L123" s="147" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="M123" s="147"/>
       <c r="N123" s="147"/>
@@ -13264,7 +13261,7 @@
       </c>
       <c r="AA123" s="158"/>
       <c r="AB123" s="158" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="AC123" s="158"/>
     </row>
@@ -13277,7 +13274,7 @@
         <v>76</v>
       </c>
       <c r="D124" s="136" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="E124" s="131" t="s">
         <v>232</v>
@@ -13286,7 +13283,7 @@
         <v>130</v>
       </c>
       <c r="G124" s="142" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="H124" s="143">
         <v>74263</v>
@@ -13331,7 +13328,7 @@
       </c>
       <c r="AA124" s="158"/>
       <c r="AB124" s="158" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="AC124" s="158"/>
     </row>
@@ -13344,28 +13341,28 @@
         <v>76</v>
       </c>
       <c r="D125" s="136" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="E125" s="131" t="s">
         <v>61</v>
       </c>
       <c r="F125" s="137" t="s">
-        <v>1080</v>
+        <v>78</v>
       </c>
       <c r="G125" s="142" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="H125" s="143">
         <v>74398</v>
       </c>
       <c r="I125" s="147" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="J125" s="147" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="K125" s="147" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="L125" s="147"/>
       <c r="M125" s="147"/>
@@ -13398,7 +13395,7 @@
       </c>
       <c r="AA125" s="158"/>
       <c r="AB125" s="158" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="AC125" s="158"/>
     </row>
@@ -13411,16 +13408,16 @@
         <v>76</v>
       </c>
       <c r="D126" s="136" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="E126" s="131" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="F126" s="137" t="s">
         <v>502</v>
       </c>
       <c r="G126" s="142" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="H126" s="143">
         <v>74947</v>
@@ -13463,7 +13460,7 @@
       </c>
       <c r="AA126" s="158"/>
       <c r="AB126" s="158" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="AC126" s="158"/>
     </row>
@@ -13474,22 +13471,22 @@
       <c r="B127" s="132"/>
       <c r="C127" s="133"/>
       <c r="D127" s="136" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="E127" s="131" t="s">
         <v>574</v>
       </c>
       <c r="F127" s="137" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="G127" s="142" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="H127" s="143">
         <v>74999</v>
       </c>
       <c r="I127" s="147" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="J127" s="147" t="s">
         <v>578</v>
@@ -13528,7 +13525,7 @@
       </c>
       <c r="AA127" s="158"/>
       <c r="AB127" s="158" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="AC127" s="158"/>
     </row>
@@ -13541,22 +13538,22 @@
         <v>76</v>
       </c>
       <c r="D128" s="136" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="E128" s="131" t="s">
         <v>570</v>
       </c>
       <c r="F128" s="137" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="G128" s="142" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="H128" s="143">
         <v>75050</v>
       </c>
       <c r="I128" s="147" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="J128" s="147"/>
       <c r="K128" s="147"/>
@@ -13591,7 +13588,7 @@
       </c>
       <c r="AA128" s="158"/>
       <c r="AB128" s="158" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="AC128" s="158"/>
     </row>
@@ -13630,31 +13627,31 @@
         <v>1</v>
       </c>
       <c r="B1" s="90" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C1" s="90">
         <v>15</v>
       </c>
       <c r="D1" s="90" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E1" s="90">
         <v>29</v>
       </c>
       <c r="F1" s="90" t="s">
+        <v>711</v>
+      </c>
+      <c r="G1" s="90">
+        <v>43</v>
+      </c>
+      <c r="H1" s="90" t="s">
         <v>712</v>
-      </c>
-      <c r="G1" s="90">
-        <v>43</v>
-      </c>
-      <c r="H1" s="90" t="s">
-        <v>713</v>
       </c>
       <c r="I1" s="90">
         <v>57</v>
       </c>
       <c r="J1" s="90" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -13662,31 +13659,31 @@
         <v>2</v>
       </c>
       <c r="B2" s="90" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C2" s="90">
         <v>16</v>
       </c>
       <c r="D2" s="90" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E2" s="90">
         <v>30</v>
       </c>
       <c r="F2" s="90" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G2" s="90">
         <v>44</v>
       </c>
       <c r="H2" s="90" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I2" s="90">
         <v>58</v>
       </c>
       <c r="J2" s="90" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -13694,25 +13691,25 @@
         <v>3</v>
       </c>
       <c r="B3" s="90" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C3" s="90">
         <v>17</v>
       </c>
       <c r="D3" s="90" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E3" s="90">
         <v>31</v>
       </c>
       <c r="F3" s="90" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G3" s="90">
         <v>45</v>
       </c>
       <c r="H3" s="90" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I3" s="91"/>
       <c r="J3" s="91"/>
@@ -13722,25 +13719,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C4" s="90">
         <v>18</v>
       </c>
       <c r="D4" s="90" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E4" s="90">
         <v>32</v>
       </c>
       <c r="F4" s="90" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G4" s="90">
         <v>46</v>
       </c>
       <c r="H4" s="90" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I4" s="91"/>
       <c r="J4" s="91"/>
@@ -13750,25 +13747,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="90" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C5" s="90">
         <v>19</v>
       </c>
       <c r="D5" s="90" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E5" s="90">
         <v>33</v>
       </c>
       <c r="F5" s="90" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G5" s="90">
         <v>47</v>
       </c>
       <c r="H5" s="90" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I5" s="91"/>
       <c r="J5" s="91"/>
@@ -13778,25 +13775,25 @@
         <v>6</v>
       </c>
       <c r="B6" s="90" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C6" s="90">
         <v>20</v>
       </c>
       <c r="D6" s="90" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E6" s="90">
         <v>34</v>
       </c>
       <c r="F6" s="90" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G6" s="90">
         <v>48</v>
       </c>
       <c r="H6" s="90" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I6" s="91"/>
       <c r="J6" s="91"/>
@@ -13806,25 +13803,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="90" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C7" s="90">
         <v>21</v>
       </c>
       <c r="D7" s="90" t="s">
+        <v>736</v>
+      </c>
+      <c r="E7" s="90">
+        <v>35</v>
+      </c>
+      <c r="F7" s="90" t="s">
         <v>737</v>
-      </c>
-      <c r="E7" s="90">
-        <v>35</v>
-      </c>
-      <c r="F7" s="90" t="s">
-        <v>738</v>
       </c>
       <c r="G7" s="90">
         <v>49</v>
       </c>
       <c r="H7" s="90" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I7" s="91"/>
       <c r="J7" s="91"/>
@@ -13834,25 +13831,25 @@
         <v>8</v>
       </c>
       <c r="B8" s="90" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C8" s="90">
         <v>22</v>
       </c>
       <c r="D8" s="90" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E8" s="90">
         <v>36</v>
       </c>
       <c r="F8" s="90" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G8" s="90">
         <v>50</v>
       </c>
       <c r="H8" s="90" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I8" s="91"/>
       <c r="J8" s="91"/>
@@ -13862,25 +13859,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C9" s="90">
         <v>23</v>
       </c>
       <c r="D9" s="90" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E9" s="90">
         <v>37</v>
       </c>
       <c r="F9" s="90" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="G9" s="90">
         <v>51</v>
       </c>
       <c r="H9" s="90" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="I9" s="91"/>
       <c r="J9" s="91"/>
@@ -13890,25 +13887,25 @@
         <v>10</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C10" s="90">
         <v>24</v>
       </c>
       <c r="D10" s="90" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E10" s="90">
         <v>38</v>
       </c>
       <c r="F10" s="90" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G10" s="90">
         <v>52</v>
       </c>
       <c r="H10" s="90" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I10" s="91"/>
       <c r="J10" s="91"/>
@@ -13918,25 +13915,25 @@
         <v>11</v>
       </c>
       <c r="B11" s="90" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C11" s="90">
         <v>25</v>
       </c>
       <c r="D11" s="90" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E11" s="90">
         <v>39</v>
       </c>
       <c r="F11" s="90" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G11" s="90">
         <v>53</v>
       </c>
       <c r="H11" s="90" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I11" s="91"/>
       <c r="J11" s="91"/>
@@ -13946,25 +13943,25 @@
         <v>12</v>
       </c>
       <c r="B12" s="90" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C12" s="90">
         <v>26</v>
       </c>
       <c r="D12" s="90" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E12" s="90">
         <v>40</v>
       </c>
       <c r="F12" s="90" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G12" s="90">
         <v>54</v>
       </c>
       <c r="H12" s="90" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I12" s="91"/>
       <c r="J12" s="91"/>
@@ -13974,25 +13971,25 @@
         <v>13</v>
       </c>
       <c r="B13" s="90" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C13" s="90">
         <v>27</v>
       </c>
       <c r="D13" s="90" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E13" s="90">
         <v>41</v>
       </c>
       <c r="F13" s="90" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G13" s="90">
         <v>55</v>
       </c>
       <c r="H13" s="90" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="I13" s="91"/>
       <c r="J13" s="91"/>
@@ -14002,25 +13999,25 @@
         <v>14</v>
       </c>
       <c r="B14" s="90" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C14" s="90">
         <v>28</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E14" s="90">
         <v>42</v>
       </c>
       <c r="F14" s="90" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G14" s="90">
         <v>56</v>
       </c>
       <c r="H14" s="90" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="I14" s="91"/>
       <c r="J14" s="91"/>
@@ -14084,13 +14081,13 @@
         <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F2" s="64" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G2" s="7">
         <v>49957</v>
@@ -14107,7 +14104,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>40</v>
@@ -14153,7 +14150,7 @@
         <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>46</v>
@@ -14176,7 +14173,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>53</v>
@@ -14199,7 +14196,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>60</v>
@@ -14222,7 +14219,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>66</v>
@@ -14241,7 +14238,7 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>71</v>
@@ -14264,7 +14261,7 @@
         <v>76</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>78</v>
@@ -14566,7 +14563,7 @@
         <v>163</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F23" s="64" t="s">
         <v>165</v>
@@ -15041,7 +15038,7 @@
         <v>289</v>
       </c>
       <c r="E44" s="71" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F44" s="69" t="s">
         <v>291</v>
@@ -15079,7 +15076,7 @@
         <v>311</v>
       </c>
       <c r="E46" s="71" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F46" s="69" t="s">
         <v>312</v>
@@ -15133,7 +15130,7 @@
       <c r="B49" s="22"/>
       <c r="C49" s="21"/>
       <c r="D49" s="22" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E49" s="21" t="s">
         <v>172</v>
@@ -15152,7 +15149,7 @@
       <c r="B50" s="19"/>
       <c r="C50" s="18"/>
       <c r="D50" s="19" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E50" s="68" t="s">
         <v>336</v>
@@ -15171,7 +15168,7 @@
       <c r="B51" s="22"/>
       <c r="C51" s="21"/>
       <c r="D51" s="22" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E51" s="21" t="s">
         <v>248</v>
@@ -15284,7 +15281,7 @@
       </c>
       <c r="B57" s="29"/>
       <c r="D57" s="30" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E57" s="73" t="s">
         <v>325</v>
@@ -15302,7 +15299,7 @@
       </c>
       <c r="B58" s="29"/>
       <c r="D58" s="32" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E58" s="75" t="s">
         <v>297</v>
@@ -15321,7 +15318,7 @@
       <c r="B59" s="27"/>
       <c r="C59" s="28"/>
       <c r="D59" s="30" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E59" s="77" t="s">
         <v>404</v>
@@ -15340,7 +15337,7 @@
       <c r="B60" s="27"/>
       <c r="C60" s="28"/>
       <c r="D60" s="32" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E60" s="79" t="s">
         <v>412</v>
@@ -15359,7 +15356,7 @@
       <c r="B61" s="27"/>
       <c r="C61" s="28"/>
       <c r="D61" s="30" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E61" s="77" t="s">
         <v>418</v>
@@ -15378,7 +15375,7 @@
       <c r="B62" s="27"/>
       <c r="C62" s="28"/>
       <c r="D62" s="32" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E62" s="79" t="s">
         <v>425</v>
@@ -15397,7 +15394,7 @@
       <c r="B63" s="36"/>
       <c r="C63" s="37"/>
       <c r="D63" s="30" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E63" s="77" t="s">
         <v>432</v>
@@ -15416,7 +15413,7 @@
       <c r="B64" s="27"/>
       <c r="C64" s="28"/>
       <c r="D64" s="32" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E64" s="79" t="s">
         <v>96</v>
@@ -15435,10 +15432,10 @@
       <c r="B65" s="38"/>
       <c r="C65" s="39"/>
       <c r="D65" s="40" t="s">
+        <v>789</v>
+      </c>
+      <c r="E65" s="77" t="s">
         <v>790</v>
-      </c>
-      <c r="E65" s="77" t="s">
-        <v>791</v>
       </c>
       <c r="F65" s="78" t="s">
         <v>444</v>
@@ -15454,10 +15451,10 @@
       <c r="B66" s="27"/>
       <c r="C66" s="28"/>
       <c r="D66" s="41" t="s">
+        <v>791</v>
+      </c>
+      <c r="E66" s="79" t="s">
         <v>792</v>
-      </c>
-      <c r="E66" s="79" t="s">
-        <v>793</v>
       </c>
       <c r="F66" s="80" t="s">
         <v>448</v>
@@ -15473,7 +15470,7 @@
       <c r="B67" s="27"/>
       <c r="C67" s="28"/>
       <c r="D67" s="40" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E67" s="77" t="s">
         <v>453</v>
@@ -15492,7 +15489,7 @@
       <c r="B68" s="43"/>
       <c r="C68" s="44"/>
       <c r="D68" s="41" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E68" s="79" t="s">
         <v>459</v>
@@ -15511,7 +15508,7 @@
       <c r="B69" s="47"/>
       <c r="C69" s="48"/>
       <c r="D69" s="40" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E69" s="77" t="s">
         <v>274</v>
@@ -15530,10 +15527,10 @@
       <c r="B70" s="27"/>
       <c r="C70" s="28"/>
       <c r="D70" s="50" t="s">
+        <v>796</v>
+      </c>
+      <c r="E70" s="81" t="s">
         <v>797</v>
-      </c>
-      <c r="E70" s="81" t="s">
-        <v>798</v>
       </c>
       <c r="F70" s="82" t="s">
         <v>471</v>
@@ -15552,7 +15549,7 @@
         <v>476</v>
       </c>
       <c r="E71" s="83" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F71" s="83" t="s">
         <v>478</v>
@@ -15571,7 +15568,7 @@
         <v>487</v>
       </c>
       <c r="E72" s="83" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F72" s="78" t="s">
         <v>488</v>
@@ -15582,7 +15579,7 @@
     </row>
     <row r="73" spans="1:7" ht="28.8">
       <c r="A73" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B73" s="54"/>
       <c r="C73" s="54"/>
@@ -15601,7 +15598,7 @@
     </row>
     <row r="74" spans="1:7" ht="28.8">
       <c r="A74" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B74" s="57"/>
       <c r="C74" s="54"/>
@@ -15620,7 +15617,7 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B75" s="60"/>
       <c r="C75" s="61"/>
@@ -15639,7 +15636,7 @@
     </row>
     <row r="76" spans="1:7" ht="43.2">
       <c r="A76" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B76" s="57"/>
       <c r="C76" s="54"/>
@@ -15658,7 +15655,7 @@
     </row>
     <row r="77" spans="1:7" ht="28.8">
       <c r="A77" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B77" s="29"/>
       <c r="D77" s="55" t="s">
@@ -15676,7 +15673,7 @@
     </row>
     <row r="78" spans="1:7" ht="28.8">
       <c r="A78" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D78" s="58" t="s">
         <v>527</v>
@@ -15693,7 +15690,7 @@
     </row>
     <row r="79" spans="1:7" ht="28.8">
       <c r="A79" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B79" s="29"/>
       <c r="D79" s="55" t="s">
@@ -15711,14 +15708,14 @@
     </row>
     <row r="80" spans="1:7" ht="28.8">
       <c r="A80" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B80" s="29"/>
       <c r="D80" s="58" t="s">
         <v>537</v>
       </c>
       <c r="E80" s="59" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F80" s="59" t="s">
         <v>539</v>
@@ -15729,7 +15726,7 @@
     </row>
     <row r="81" spans="1:7" ht="28.8">
       <c r="A81" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B81" s="29"/>
       <c r="D81" s="55" t="s">
@@ -15747,7 +15744,7 @@
     </row>
     <row r="82" spans="1:7" ht="43.2">
       <c r="A82" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B82" s="29"/>
       <c r="D82" s="58" t="s">
@@ -15765,7 +15762,7 @@
     </row>
     <row r="83" spans="1:7" ht="28.8">
       <c r="A83" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B83" s="29"/>
       <c r="D83" s="55" t="s">
@@ -15783,7 +15780,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B84" s="29"/>
       <c r="D84" s="58" t="s">
@@ -15801,7 +15798,7 @@
     </row>
     <row r="85" spans="1:7" ht="28.8">
       <c r="A85" s="54" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="B85" s="29"/>
       <c r="D85" s="55" t="s">
@@ -15940,16 +15937,16 @@
         <v>2014</v>
       </c>
       <c r="C2" s="86" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2" s="86" t="s">
         <v>802</v>
-      </c>
-      <c r="D2" s="86" t="s">
-        <v>803</v>
       </c>
       <c r="E2" s="86" t="s">
         <v>118</v>
       </c>
       <c r="F2" s="86" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G2" s="86">
         <v>45467</v>
@@ -15960,13 +15957,13 @@
         <v>2014</v>
       </c>
       <c r="C3" s="86" t="s">
+        <v>804</v>
+      </c>
+      <c r="D3" s="86" t="s">
         <v>805</v>
       </c>
-      <c r="D3" s="86" t="s">
+      <c r="F3" s="86" t="s">
         <v>806</v>
-      </c>
-      <c r="F3" s="86" t="s">
-        <v>807</v>
       </c>
       <c r="G3" s="86">
         <v>30904</v>
@@ -15977,16 +15974,16 @@
         <v>2014</v>
       </c>
       <c r="C4" s="86" t="s">
+        <v>807</v>
+      </c>
+      <c r="D4" s="86" t="s">
         <v>808</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="E4" s="86" t="s">
         <v>809</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="F4" s="86" t="s">
         <v>810</v>
-      </c>
-      <c r="F4" s="86" t="s">
-        <v>811</v>
       </c>
       <c r="G4" s="86">
         <v>41324</v>
@@ -15997,25 +15994,25 @@
         <v>2014</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D5" s="86" t="s">
         <v>513</v>
       </c>
       <c r="E5" s="86" t="s">
+        <v>812</v>
+      </c>
+      <c r="F5" s="86" t="s">
         <v>813</v>
-      </c>
-      <c r="F5" s="86" t="s">
-        <v>814</v>
       </c>
       <c r="G5" s="86">
         <v>101047</v>
       </c>
       <c r="H5" s="86" t="s">
+        <v>814</v>
+      </c>
+      <c r="I5" s="86" t="s">
         <v>815</v>
-      </c>
-      <c r="I5" s="86" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="6" spans="1:25">
@@ -16023,7 +16020,7 @@
         <v>2014</v>
       </c>
       <c r="C6" s="86" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D6" s="86" t="s">
         <v>156</v>
@@ -16032,7 +16029,7 @@
         <v>172</v>
       </c>
       <c r="F6" s="86" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G6" s="86">
         <v>60020</v>
@@ -16046,7 +16043,7 @@
         <v>2014</v>
       </c>
       <c r="C7" s="86" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D7" s="86" t="s">
         <v>31</v>
@@ -16055,7 +16052,7 @@
         <v>331</v>
       </c>
       <c r="F7" s="86" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G7" s="86">
         <v>49993</v>
@@ -16069,13 +16066,13 @@
         <v>2014</v>
       </c>
       <c r="C8" s="86" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D8" s="86" t="s">
         <v>135</v>
       </c>
       <c r="F8" s="86" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G8" s="86">
         <v>49247</v>
@@ -16086,7 +16083,7 @@
         <v>2014</v>
       </c>
       <c r="C9" s="86" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D9" s="86" t="s">
         <v>40</v>
@@ -16095,7 +16092,7 @@
         <v>41</v>
       </c>
       <c r="F9" s="86" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G9" s="86">
         <v>48909</v>
@@ -16106,16 +16103,16 @@
         <v>2014</v>
       </c>
       <c r="C10" s="86" t="s">
+        <v>824</v>
+      </c>
+      <c r="D10" s="86" t="s">
         <v>825</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="E10" s="86" t="s">
         <v>826</v>
       </c>
-      <c r="E10" s="86" t="s">
+      <c r="F10" s="86" t="s">
         <v>827</v>
-      </c>
-      <c r="F10" s="86" t="s">
-        <v>828</v>
       </c>
       <c r="G10" s="86">
         <v>50000</v>
@@ -16126,22 +16123,22 @@
         <v>2014</v>
       </c>
       <c r="C11" s="86" t="s">
+        <v>828</v>
+      </c>
+      <c r="D11" s="86" t="s">
         <v>829</v>
-      </c>
-      <c r="D11" s="86" t="s">
-        <v>830</v>
       </c>
       <c r="E11" s="86" t="s">
         <v>96</v>
       </c>
       <c r="F11" s="86" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="G11" s="86">
         <v>96000</v>
       </c>
       <c r="H11" s="86" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="12" spans="1:25">
@@ -16149,16 +16146,16 @@
         <v>2014</v>
       </c>
       <c r="C12" s="86" t="s">
+        <v>832</v>
+      </c>
+      <c r="D12" s="86" t="s">
+        <v>808</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>809</v>
+      </c>
+      <c r="F12" s="86" t="s">
         <v>833</v>
-      </c>
-      <c r="D12" s="86" t="s">
-        <v>809</v>
-      </c>
-      <c r="E12" s="86" t="s">
-        <v>810</v>
-      </c>
-      <c r="F12" s="86" t="s">
-        <v>834</v>
       </c>
       <c r="G12" s="86">
         <v>49906</v>
@@ -16172,16 +16169,16 @@
         <v>29</v>
       </c>
       <c r="C13" s="86" t="s">
+        <v>834</v>
+      </c>
+      <c r="D13" s="86" t="s">
         <v>835</v>
       </c>
-      <c r="D13" s="86" t="s">
+      <c r="E13" s="86" t="s">
         <v>836</v>
       </c>
-      <c r="E13" s="86" t="s">
+      <c r="F13" s="86" t="s">
         <v>837</v>
-      </c>
-      <c r="F13" s="86" t="s">
-        <v>838</v>
       </c>
       <c r="G13" s="86">
         <v>50000</v>
@@ -16195,7 +16192,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="86" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D14" s="86" t="s">
         <v>206</v>
@@ -16204,7 +16201,7 @@
         <v>208</v>
       </c>
       <c r="F14" s="86" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="H14" s="86" t="s">
         <v>210</v>
@@ -16218,16 +16215,16 @@
         <v>29</v>
       </c>
       <c r="C15" s="86" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D15" s="86" t="s">
         <v>181</v>
       </c>
       <c r="E15" s="86" t="s">
+        <v>841</v>
+      </c>
+      <c r="F15" s="86" t="s">
         <v>842</v>
-      </c>
-      <c r="F15" s="86" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="16" spans="1:25">
@@ -16241,7 +16238,7 @@
         <v>388</v>
       </c>
       <c r="F16" s="86" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -16255,16 +16252,16 @@
         <v>40</v>
       </c>
       <c r="E17" s="86" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F17" s="86" t="s">
         <v>312</v>
       </c>
       <c r="H17" s="86" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="I17" s="86" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -16275,10 +16272,10 @@
         <v>29</v>
       </c>
       <c r="D18" s="86" t="s">
+        <v>846</v>
+      </c>
+      <c r="F18" s="86" t="s">
         <v>847</v>
-      </c>
-      <c r="F18" s="86" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -16289,7 +16286,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="86" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D19" s="86" t="s">
         <v>268</v>
@@ -16298,7 +16295,7 @@
         <v>145</v>
       </c>
       <c r="F19" s="86" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G19" s="86">
         <v>69960</v>
@@ -16315,7 +16312,7 @@
         <v>29</v>
       </c>
       <c r="C20" s="86" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D20" s="86" t="s">
         <v>172</v>
@@ -16324,7 +16321,7 @@
         <v>331</v>
       </c>
       <c r="F20" s="86" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G20" s="86">
         <v>76098</v>
@@ -16373,19 +16370,19 @@
         <v>29</v>
       </c>
       <c r="C22" s="86" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="D22" s="86" t="s">
         <v>145</v>
       </c>
       <c r="E22" s="86" t="s">
+        <v>853</v>
+      </c>
+      <c r="F22" s="86" t="s">
         <v>854</v>
       </c>
-      <c r="F22" s="86" t="s">
+      <c r="H22" s="86" t="s">
         <v>855</v>
-      </c>
-      <c r="H22" s="86" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -16396,7 +16393,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="86" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D23" s="86" t="s">
         <v>208</v>
@@ -16405,7 +16402,7 @@
         <v>372</v>
       </c>
       <c r="F23" s="86" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="G23" s="86">
         <v>95834</v>
@@ -16419,25 +16416,25 @@
         <v>29</v>
       </c>
       <c r="C24" s="86" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D24" s="86" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="86" t="s">
+        <v>859</v>
+      </c>
+      <c r="F24" s="86" t="s">
         <v>860</v>
-      </c>
-      <c r="F24" s="86" t="s">
-        <v>861</v>
       </c>
       <c r="G24" s="86">
         <v>2017692</v>
       </c>
       <c r="H24" s="86" t="s">
+        <v>861</v>
+      </c>
+      <c r="I24" s="86" t="s">
         <v>862</v>
-      </c>
-      <c r="I24" s="86" t="s">
-        <v>863</v>
       </c>
       <c r="J24" s="86" t="s">
         <v>155</v>
@@ -16446,7 +16443,7 @@
         <v>280</v>
       </c>
       <c r="L24" s="86" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -16457,16 +16454,16 @@
         <v>29</v>
       </c>
       <c r="C25" s="86" t="s">
+        <v>864</v>
+      </c>
+      <c r="D25" s="86" t="s">
         <v>865</v>
       </c>
-      <c r="D25" s="86" t="s">
+      <c r="E25" s="86" t="s">
         <v>866</v>
       </c>
-      <c r="E25" s="86" t="s">
+      <c r="F25" s="86" t="s">
         <v>867</v>
-      </c>
-      <c r="F25" s="86" t="s">
-        <v>868</v>
       </c>
       <c r="G25" s="86">
         <v>91750</v>
@@ -16480,28 +16477,28 @@
         <v>29</v>
       </c>
       <c r="C26" s="86" t="s">
+        <v>868</v>
+      </c>
+      <c r="D26" s="86" t="s">
+        <v>667</v>
+      </c>
+      <c r="E26" s="86" t="s">
         <v>869</v>
       </c>
-      <c r="D26" s="86" t="s">
-        <v>668</v>
-      </c>
-      <c r="E26" s="86" t="s">
+      <c r="F26" s="86" t="s">
         <v>870</v>
-      </c>
-      <c r="F26" s="86" t="s">
-        <v>871</v>
       </c>
       <c r="G26" s="86">
         <v>109971.4</v>
       </c>
       <c r="H26" s="86" t="s">
+        <v>871</v>
+      </c>
+      <c r="I26" s="86" t="s">
         <v>872</v>
       </c>
-      <c r="I26" s="86" t="s">
+      <c r="J26" s="86" t="s">
         <v>873</v>
-      </c>
-      <c r="J26" s="86" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -16512,22 +16509,22 @@
         <v>29</v>
       </c>
       <c r="C27" s="86" t="s">
+        <v>874</v>
+      </c>
+      <c r="D27" s="86" t="s">
         <v>875</v>
       </c>
-      <c r="D27" s="86" t="s">
+      <c r="E27" s="86" t="s">
         <v>876</v>
       </c>
-      <c r="E27" s="86" t="s">
+      <c r="F27" s="86" t="s">
         <v>877</v>
-      </c>
-      <c r="F27" s="86" t="s">
-        <v>878</v>
       </c>
       <c r="G27" s="86">
         <v>78679</v>
       </c>
       <c r="H27" s="86" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I27" s="86" t="s">
         <v>284</v>
@@ -16541,16 +16538,16 @@
         <v>29</v>
       </c>
       <c r="C28" s="86" t="s">
+        <v>878</v>
+      </c>
+      <c r="D28" s="86" t="s">
         <v>879</v>
       </c>
-      <c r="D28" s="86" t="s">
+      <c r="E28" s="86" t="s">
+        <v>844</v>
+      </c>
+      <c r="F28" s="86" t="s">
         <v>880</v>
-      </c>
-      <c r="E28" s="86" t="s">
-        <v>845</v>
-      </c>
-      <c r="F28" s="86" t="s">
-        <v>881</v>
       </c>
       <c r="G28" s="86">
         <v>54871</v>
@@ -16567,22 +16564,22 @@
         <v>29</v>
       </c>
       <c r="C29" s="86" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D29" s="86" t="s">
         <v>284</v>
       </c>
       <c r="E29" s="86" t="s">
+        <v>882</v>
+      </c>
+      <c r="F29" s="86" t="s">
         <v>883</v>
-      </c>
-      <c r="F29" s="86" t="s">
-        <v>884</v>
       </c>
       <c r="G29" s="86">
         <v>116779.08</v>
       </c>
       <c r="H29" s="86" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -16593,25 +16590,25 @@
         <v>29</v>
       </c>
       <c r="C30" s="86" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D30" s="86" t="s">
         <v>443</v>
       </c>
       <c r="E30" s="86" t="s">
+        <v>886</v>
+      </c>
+      <c r="F30" s="86" t="s">
         <v>887</v>
-      </c>
-      <c r="F30" s="86" t="s">
-        <v>888</v>
       </c>
       <c r="G30" s="86">
         <v>93749</v>
       </c>
       <c r="H30" s="86" t="s">
+        <v>888</v>
+      </c>
+      <c r="I30" s="86" t="s">
         <v>889</v>
-      </c>
-      <c r="I30" s="86" t="s">
-        <v>890</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -16622,7 +16619,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="86" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D31" s="86" t="s">
         <v>61</v>
@@ -16631,7 +16628,7 @@
         <v>78</v>
       </c>
       <c r="F31" s="86" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G31" s="86">
         <v>13503</v>
@@ -16645,7 +16642,7 @@
         <v>29</v>
       </c>
       <c r="C32" s="86" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="D32" s="86" t="s">
         <v>344</v>
@@ -16654,7 +16651,7 @@
         <v>248</v>
       </c>
       <c r="F32" s="86" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G32" s="86">
         <v>129304</v>
@@ -16663,7 +16660,7 @@
         <v>555</v>
       </c>
       <c r="I32" s="86" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J32" s="86" t="s">
         <v>346</v>
@@ -16677,16 +16674,16 @@
         <v>29</v>
       </c>
       <c r="C33" s="86" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D33" s="86" t="s">
         <v>185</v>
       </c>
       <c r="E33" s="86" t="s">
+        <v>896</v>
+      </c>
+      <c r="F33" s="86" t="s">
         <v>897</v>
-      </c>
-      <c r="F33" s="86" t="s">
-        <v>898</v>
       </c>
       <c r="G33" s="86">
         <v>65084</v>
@@ -16695,7 +16692,7 @@
         <v>501</v>
       </c>
       <c r="I33" s="86" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -16706,7 +16703,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="86" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D34" s="86" t="s">
         <v>284</v>
@@ -16715,7 +16712,7 @@
         <v>185</v>
       </c>
       <c r="F34" s="86" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G34" s="86">
         <v>120009.5</v>
@@ -16727,7 +16724,7 @@
         <v>139</v>
       </c>
       <c r="J34" s="86" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -16738,22 +16735,22 @@
         <v>29</v>
       </c>
       <c r="C35" s="86" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D35" s="86" t="s">
         <v>215</v>
       </c>
       <c r="E35" s="86" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F35" s="86" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G35" s="86">
         <v>50000</v>
       </c>
       <c r="H35" s="86" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -16764,22 +16761,22 @@
         <v>29</v>
       </c>
       <c r="C36" s="86" t="s">
+        <v>905</v>
+      </c>
+      <c r="D36" s="86" t="s">
         <v>906</v>
       </c>
-      <c r="D36" s="86" t="s">
+      <c r="E36" s="86" t="s">
         <v>907</v>
       </c>
-      <c r="E36" s="86" t="s">
+      <c r="F36" s="86" t="s">
         <v>908</v>
-      </c>
-      <c r="F36" s="86" t="s">
-        <v>909</v>
       </c>
       <c r="G36" s="86">
         <v>59656</v>
       </c>
       <c r="H36" s="86" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="I36" s="86" t="s">
         <v>534</v>
@@ -16796,22 +16793,22 @@
         <v>29</v>
       </c>
       <c r="C37" s="86" t="s">
+        <v>910</v>
+      </c>
+      <c r="D37" s="86" t="s">
         <v>911</v>
-      </c>
-      <c r="D37" s="86" t="s">
-        <v>912</v>
       </c>
       <c r="E37" s="86" t="s">
         <v>585</v>
       </c>
       <c r="F37" s="86" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G37" s="86">
         <v>56518</v>
       </c>
       <c r="H37" s="86" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I37" s="86" t="s">
         <v>347</v>
@@ -16825,16 +16822,16 @@
         <v>29</v>
       </c>
       <c r="C38" s="86" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D38" s="86" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E38" s="86" t="s">
         <v>555</v>
       </c>
       <c r="F38" s="86" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="G38" s="86">
         <v>45977</v>
@@ -16848,16 +16845,16 @@
         <v>29</v>
       </c>
       <c r="C39" s="86" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D39" s="86" t="s">
         <v>185</v>
       </c>
       <c r="E39" s="86" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="F39" s="86" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G39" s="86">
         <v>81229</v>
@@ -16874,16 +16871,16 @@
         <v>29</v>
       </c>
       <c r="C40" s="86" t="s">
+        <v>917</v>
+      </c>
+      <c r="D40" s="86" t="s">
         <v>918</v>
       </c>
-      <c r="D40" s="86" t="s">
+      <c r="E40" s="86" t="s">
         <v>919</v>
       </c>
-      <c r="E40" s="86" t="s">
+      <c r="F40" s="86" t="s">
         <v>920</v>
-      </c>
-      <c r="F40" s="86" t="s">
-        <v>921</v>
       </c>
       <c r="G40" s="86">
         <v>50000</v>
@@ -16906,7 +16903,7 @@
         <v>29</v>
       </c>
       <c r="C41" s="86" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D41" s="86" t="s">
         <v>185</v>
@@ -16915,7 +16912,7 @@
         <v>248</v>
       </c>
       <c r="F41" s="86" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G41" s="86">
         <v>69482</v>
@@ -16935,22 +16932,22 @@
         <v>29</v>
       </c>
       <c r="C42" s="86" t="s">
+        <v>923</v>
+      </c>
+      <c r="D42" s="86" t="s">
         <v>924</v>
       </c>
-      <c r="D42" s="86" t="s">
+      <c r="E42" s="86" t="s">
         <v>925</v>
       </c>
-      <c r="E42" s="86" t="s">
+      <c r="F42" s="86" t="s">
         <v>926</v>
-      </c>
-      <c r="F42" s="86" t="s">
-        <v>927</v>
       </c>
       <c r="G42" s="86">
         <v>118402.42</v>
       </c>
       <c r="H42" s="86" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="I42" s="86" t="s">
         <v>372</v>
@@ -16970,7 +16967,7 @@
         <v>29</v>
       </c>
       <c r="C43" s="86" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D43" s="86" t="s">
         <v>284</v>
@@ -16979,16 +16976,16 @@
         <v>185</v>
       </c>
       <c r="F43" s="86" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="G43" s="86">
         <v>59605</v>
       </c>
       <c r="H43" s="86" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I43" s="86" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -16999,16 +16996,16 @@
         <v>29</v>
       </c>
       <c r="C44" s="86" t="s">
+        <v>931</v>
+      </c>
+      <c r="D44" s="86" t="s">
+        <v>865</v>
+      </c>
+      <c r="E44" s="86" t="s">
         <v>932</v>
       </c>
-      <c r="D44" s="86" t="s">
-        <v>866</v>
-      </c>
-      <c r="E44" s="86" t="s">
+      <c r="F44" s="86" t="s">
         <v>933</v>
-      </c>
-      <c r="F44" s="86" t="s">
-        <v>934</v>
       </c>
       <c r="G44" s="86">
         <v>74869</v>
@@ -17025,28 +17022,28 @@
         <v>29</v>
       </c>
       <c r="C45" s="86" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D45" s="86" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E45" s="86" t="s">
         <v>443</v>
       </c>
       <c r="F45" s="86" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="G45" s="87">
         <v>126310.39999999999</v>
       </c>
       <c r="H45" s="86" t="s">
+        <v>936</v>
+      </c>
+      <c r="I45" s="86" t="s">
         <v>937</v>
       </c>
-      <c r="I45" s="86" t="s">
-        <v>938</v>
-      </c>
       <c r="J45" s="86" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="K45" s="86" t="s">
         <v>492</v>
@@ -17060,7 +17057,7 @@
         <v>29</v>
       </c>
       <c r="C46" s="86" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D46" s="86" t="s">
         <v>347</v>
@@ -17069,7 +17066,7 @@
         <v>532</v>
       </c>
       <c r="F46" s="86" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="G46" s="86">
         <v>81357</v>
@@ -17083,7 +17080,7 @@
         <v>29</v>
       </c>
       <c r="C47" s="86" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D47" s="86" t="s">
         <v>574</v>
@@ -17092,7 +17089,7 @@
         <v>578</v>
       </c>
       <c r="F47" s="86" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G47" s="86">
         <v>77807</v>
@@ -17112,22 +17109,22 @@
         <v>76</v>
       </c>
       <c r="C48" s="86" t="s">
+        <v>942</v>
+      </c>
+      <c r="D48" s="86" t="s">
         <v>943</v>
-      </c>
-      <c r="D48" s="86" t="s">
-        <v>944</v>
       </c>
       <c r="E48" s="86" t="s">
         <v>284</v>
       </c>
       <c r="F48" s="86" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G48" s="86">
         <v>75000</v>
       </c>
       <c r="H48" s="86" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="I48" s="86" t="s">
         <v>331</v>
@@ -17141,40 +17138,40 @@
         <v>76</v>
       </c>
       <c r="C49" s="86" t="s">
+        <v>946</v>
+      </c>
+      <c r="D49" s="86" t="s">
         <v>947</v>
       </c>
-      <c r="D49" s="86" t="s">
+      <c r="E49" s="86" t="s">
         <v>948</v>
       </c>
-      <c r="E49" s="86" t="s">
+      <c r="F49" s="86" t="s">
         <v>949</v>
-      </c>
-      <c r="F49" s="86" t="s">
-        <v>950</v>
       </c>
       <c r="G49" s="86">
         <v>40820</v>
       </c>
       <c r="H49" s="86" t="s">
+        <v>950</v>
+      </c>
+      <c r="I49" s="86" t="s">
         <v>951</v>
       </c>
-      <c r="I49" s="86" t="s">
+      <c r="J49" s="86" t="s">
         <v>952</v>
       </c>
-      <c r="J49" s="86" t="s">
+      <c r="K49" s="86" t="s">
         <v>953</v>
       </c>
-      <c r="K49" s="86" t="s">
+      <c r="L49" s="86" t="s">
         <v>954</v>
       </c>
-      <c r="L49" s="86" t="s">
+      <c r="M49" s="86" t="s">
         <v>955</v>
       </c>
-      <c r="M49" s="86" t="s">
+      <c r="N49" s="86" t="s">
         <v>956</v>
-      </c>
-      <c r="N49" s="86" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -17185,7 +17182,7 @@
         <v>76</v>
       </c>
       <c r="C50" s="86" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D50" s="86" t="s">
         <v>206</v>
@@ -17194,7 +17191,7 @@
         <v>208</v>
       </c>
       <c r="F50" s="86" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G50" s="86">
         <v>70000</v>
@@ -17206,7 +17203,7 @@
         <v>211</v>
       </c>
       <c r="J50" s="86" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -17217,7 +17214,7 @@
         <v>76</v>
       </c>
       <c r="C51" s="86" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="D51" s="86" t="s">
         <v>568</v>
@@ -17226,13 +17223,13 @@
         <v>135</v>
       </c>
       <c r="F51" s="86" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G51" s="86">
         <v>75250</v>
       </c>
       <c r="H51" s="86" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I51" s="86" t="s">
         <v>136</v>
@@ -17246,31 +17243,31 @@
         <v>76</v>
       </c>
       <c r="C52" s="86" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="D52" s="86" t="s">
         <v>348</v>
       </c>
       <c r="E52" s="86" t="s">
+        <v>963</v>
+      </c>
+      <c r="F52" s="86" t="s">
         <v>964</v>
-      </c>
-      <c r="F52" s="86" t="s">
-        <v>965</v>
       </c>
       <c r="G52" s="86">
         <v>75000</v>
       </c>
       <c r="H52" s="86" t="s">
+        <v>965</v>
+      </c>
+      <c r="I52" s="86" t="s">
         <v>966</v>
       </c>
-      <c r="I52" s="86" t="s">
+      <c r="J52" s="86" t="s">
         <v>967</v>
       </c>
-      <c r="J52" s="86" t="s">
-        <v>968</v>
-      </c>
       <c r="K52" s="86" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -17281,16 +17278,16 @@
         <v>76</v>
       </c>
       <c r="C53" s="86" t="s">
+        <v>968</v>
+      </c>
+      <c r="D53" s="86" t="s">
         <v>969</v>
       </c>
-      <c r="D53" s="86" t="s">
+      <c r="E53" s="86" t="s">
         <v>970</v>
       </c>
-      <c r="E53" s="86" t="s">
+      <c r="F53" s="86" t="s">
         <v>971</v>
-      </c>
-      <c r="F53" s="86" t="s">
-        <v>972</v>
       </c>
       <c r="G53" s="86">
         <v>74641</v>
@@ -17299,7 +17296,7 @@
         <v>454</v>
       </c>
       <c r="I53" s="86" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -17310,7 +17307,7 @@
         <v>76</v>
       </c>
       <c r="C54" s="86" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="D54" s="86" t="s">
         <v>245</v>
@@ -17319,7 +17316,7 @@
         <v>247</v>
       </c>
       <c r="F54" s="86" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G54" s="86">
         <v>75000</v>
@@ -17336,7 +17333,7 @@
         <v>76</v>
       </c>
       <c r="C55" s="86" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D55" s="86" t="s">
         <v>347</v>
@@ -17345,13 +17342,13 @@
         <v>585</v>
       </c>
       <c r="F55" s="86" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="G55" s="88">
         <v>65704.160000000003</v>
       </c>
       <c r="H55" s="86" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I55" s="86" t="s">
         <v>300</v>
@@ -17365,16 +17362,16 @@
         <v>76</v>
       </c>
       <c r="C56" s="86" t="s">
+        <v>977</v>
+      </c>
+      <c r="D56" s="86" t="s">
         <v>978</v>
       </c>
-      <c r="D56" s="86" t="s">
+      <c r="E56" s="86" t="s">
         <v>979</v>
       </c>
-      <c r="E56" s="86" t="s">
+      <c r="F56" s="86" t="s">
         <v>980</v>
-      </c>
-      <c r="F56" s="86" t="s">
-        <v>981</v>
       </c>
       <c r="G56" s="86">
         <v>75000</v>
@@ -17394,16 +17391,16 @@
         <v>76</v>
       </c>
       <c r="C57" s="86" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D57" s="86" t="s">
         <v>61</v>
       </c>
       <c r="E57" s="86" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F57" s="86" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G57" s="86">
         <v>49500</v>
@@ -17412,7 +17409,7 @@
         <v>534</v>
       </c>
       <c r="I57" s="86" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -17423,25 +17420,25 @@
         <v>29</v>
       </c>
       <c r="C58" s="89" t="s">
+        <v>984</v>
+      </c>
+      <c r="D58" s="86" t="s">
+        <v>865</v>
+      </c>
+      <c r="E58" s="86" t="s">
         <v>985</v>
       </c>
-      <c r="D58" s="86" t="s">
-        <v>866</v>
-      </c>
-      <c r="E58" s="86" t="s">
+      <c r="F58" s="86" t="s">
         <v>986</v>
-      </c>
-      <c r="F58" s="86" t="s">
-        <v>987</v>
       </c>
       <c r="G58" s="86">
         <v>75000</v>
       </c>
       <c r="H58" s="86" t="s">
+        <v>987</v>
+      </c>
+      <c r="I58" s="86" t="s">
         <v>988</v>
-      </c>
-      <c r="I58" s="86" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -17452,22 +17449,22 @@
         <v>29</v>
       </c>
       <c r="C59" s="89" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D59" s="86" t="s">
+        <v>876</v>
+      </c>
+      <c r="E59" s="86" t="s">
+        <v>875</v>
+      </c>
+      <c r="F59" s="86" t="s">
         <v>877</v>
-      </c>
-      <c r="E59" s="86" t="s">
-        <v>876</v>
-      </c>
-      <c r="F59" s="86" t="s">
-        <v>878</v>
       </c>
       <c r="G59" s="86">
         <v>74081</v>
       </c>
       <c r="H59" s="86" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I59" s="86" t="s">
         <v>543</v>
@@ -17481,16 +17478,16 @@
         <v>29</v>
       </c>
       <c r="C60" s="89" t="s">
+        <v>990</v>
+      </c>
+      <c r="D60" s="86" t="s">
         <v>991</v>
-      </c>
-      <c r="D60" s="86" t="s">
-        <v>992</v>
       </c>
       <c r="E60" s="86" t="s">
         <v>248</v>
       </c>
       <c r="F60" s="86" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="G60" s="86">
         <v>75000</v>
@@ -17499,16 +17496,16 @@
         <v>508</v>
       </c>
       <c r="I60" s="86" t="s">
+        <v>993</v>
+      </c>
+      <c r="J60" s="86" t="s">
         <v>994</v>
       </c>
-      <c r="J60" s="86" t="s">
+      <c r="K60" s="86" t="s">
         <v>995</v>
       </c>
-      <c r="K60" s="86" t="s">
+      <c r="L60" s="86" t="s">
         <v>996</v>
-      </c>
-      <c r="L60" s="86" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -17519,7 +17516,7 @@
         <v>29</v>
       </c>
       <c r="C61" s="89" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D61" s="86" t="s">
         <v>405</v>
@@ -17528,7 +17525,7 @@
         <v>347</v>
       </c>
       <c r="F61" s="86" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="G61" s="86">
         <v>74765</v>
@@ -17545,7 +17542,7 @@
         <v>29</v>
       </c>
       <c r="C62" s="89" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D62" s="86" t="s">
         <v>570</v>
@@ -17554,7 +17551,7 @@
         <v>443</v>
       </c>
       <c r="F62" s="86" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="G62" s="86">
         <v>153805</v>
@@ -17563,13 +17560,13 @@
         <v>130</v>
       </c>
       <c r="I62" s="86" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="J62" s="86" t="s">
         <v>382</v>
       </c>
       <c r="K62" s="86" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -17580,7 +17577,7 @@
         <v>29</v>
       </c>
       <c r="C63" s="89" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D63" s="86" t="s">
         <v>221</v>
@@ -17589,7 +17586,7 @@
         <v>98</v>
       </c>
       <c r="F63" s="86" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="G63" s="86">
         <v>70084</v>
@@ -17609,28 +17606,28 @@
         <v>29</v>
       </c>
       <c r="C64" s="89" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D64" s="86" t="s">
         <v>1005</v>
       </c>
-      <c r="D64" s="86" t="s">
+      <c r="E64" s="86" t="s">
         <v>1006</v>
       </c>
-      <c r="E64" s="86" t="s">
+      <c r="F64" s="86" t="s">
         <v>1007</v>
-      </c>
-      <c r="F64" s="86" t="s">
-        <v>1008</v>
       </c>
       <c r="G64" s="86">
         <v>75000</v>
       </c>
       <c r="H64" s="86" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I64" s="86" t="s">
         <v>1009</v>
       </c>
-      <c r="I64" s="86" t="s">
+      <c r="J64" s="86" t="s">
         <v>1010</v>
-      </c>
-      <c r="J64" s="86" t="s">
-        <v>1011</v>
       </c>
     </row>
     <row r="65" spans="1:13">
@@ -17641,16 +17638,16 @@
         <v>29</v>
       </c>
       <c r="C65" s="89" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D65" s="86" t="s">
         <v>1012</v>
       </c>
-      <c r="D65" s="86" t="s">
+      <c r="E65" s="86" t="s">
         <v>1013</v>
       </c>
-      <c r="E65" s="86" t="s">
+      <c r="F65" s="86" t="s">
         <v>1014</v>
-      </c>
-      <c r="F65" s="86" t="s">
-        <v>1015</v>
       </c>
       <c r="G65" s="86">
         <v>52640</v>
@@ -17659,7 +17656,7 @@
         <v>280</v>
       </c>
       <c r="I65" s="86" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="66" spans="1:13">
@@ -17670,7 +17667,7 @@
         <v>29</v>
       </c>
       <c r="C66" s="89" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D66" s="86" t="s">
         <v>172</v>
@@ -17679,7 +17676,7 @@
         <v>331</v>
       </c>
       <c r="F66" s="86" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="G66" s="86">
         <v>162571.4</v>
@@ -17693,25 +17690,25 @@
         <v>29</v>
       </c>
       <c r="C67" s="89" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D67" s="86" t="s">
         <v>570</v>
       </c>
       <c r="E67" s="86" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F67" s="86" t="s">
         <v>1020</v>
-      </c>
-      <c r="F67" s="86" t="s">
-        <v>1021</v>
       </c>
       <c r="G67" s="86">
         <v>72618</v>
       </c>
       <c r="H67" s="86" t="s">
+        <v>1021</v>
+      </c>
+      <c r="I67" s="86" t="s">
         <v>1022</v>
-      </c>
-      <c r="I67" s="86" t="s">
-        <v>1023</v>
       </c>
     </row>
     <row r="68" spans="1:13">
@@ -17722,16 +17719,16 @@
         <v>29</v>
       </c>
       <c r="C68" s="89" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D68" s="86" t="s">
         <v>1024</v>
-      </c>
-      <c r="D68" s="86" t="s">
-        <v>1025</v>
       </c>
       <c r="E68" s="86" t="s">
         <v>556</v>
       </c>
       <c r="F68" s="86" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G68" s="86">
         <v>127756.75</v>
@@ -17748,37 +17745,37 @@
         <v>29</v>
       </c>
       <c r="C69" s="89" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D69" s="86" t="s">
         <v>1027</v>
-      </c>
-      <c r="D69" s="86" t="s">
-        <v>1028</v>
       </c>
       <c r="E69" s="86" t="s">
         <v>135</v>
       </c>
       <c r="F69" s="86" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="G69" s="86">
         <v>74802</v>
       </c>
       <c r="H69" s="86" t="s">
+        <v>1029</v>
+      </c>
+      <c r="I69" s="86" t="s">
         <v>1030</v>
-      </c>
-      <c r="I69" s="86" t="s">
-        <v>1031</v>
       </c>
       <c r="J69" s="86" t="s">
         <v>136</v>
       </c>
       <c r="K69" s="86" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="L69" s="86" t="s">
         <v>139</v>
       </c>
       <c r="M69" s="86" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -17789,16 +17786,16 @@
         <v>29</v>
       </c>
       <c r="C70" s="89" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D70" s="86" t="s">
         <v>1034</v>
-      </c>
-      <c r="D70" s="86" t="s">
-        <v>1035</v>
       </c>
       <c r="E70" s="86" t="s">
         <v>136</v>
       </c>
       <c r="F70" s="86" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="G70" s="86">
         <v>75000</v>
@@ -17807,10 +17804,10 @@
         <v>568</v>
       </c>
       <c r="I70" s="86" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J70" s="86" t="s">
         <v>1037</v>
-      </c>
-      <c r="J70" s="86" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="71" spans="1:13">
@@ -17821,22 +17818,22 @@
         <v>29</v>
       </c>
       <c r="C71" s="89" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D71" s="86" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E71" s="86" t="s">
         <v>426</v>
       </c>
       <c r="F71" s="86" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="G71" s="86">
         <v>74998</v>
       </c>
       <c r="H71" s="86" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="72" spans="1:13">
@@ -17847,16 +17844,16 @@
         <v>29</v>
       </c>
       <c r="C72" s="89" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D72" s="86" t="s">
         <v>1042</v>
-      </c>
-      <c r="D72" s="86" t="s">
-        <v>1043</v>
       </c>
       <c r="E72" s="86" t="s">
         <v>499</v>
       </c>
       <c r="F72" s="86" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G72" s="86">
         <v>68703</v>
@@ -17876,7 +17873,7 @@
         <v>29</v>
       </c>
       <c r="C73" s="89" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D73" s="86" t="s">
         <v>574</v>
@@ -17885,7 +17882,7 @@
         <v>578</v>
       </c>
       <c r="F73" s="86" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G73" s="86">
         <v>75000</v>
@@ -17897,10 +17894,10 @@
         <v>575</v>
       </c>
       <c r="J73" s="86" t="s">
+        <v>1045</v>
+      </c>
+      <c r="K73" s="86" t="s">
         <v>1046</v>
-      </c>
-      <c r="K73" s="86" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="74" spans="1:13">
@@ -17911,16 +17908,16 @@
         <v>29</v>
       </c>
       <c r="C74" s="89" t="s">
+        <v>1047</v>
+      </c>
+      <c r="D74" s="86" t="s">
         <v>1048</v>
       </c>
-      <c r="D74" s="86" t="s">
+      <c r="E74" s="86" t="s">
         <v>1049</v>
       </c>
-      <c r="E74" s="86" t="s">
+      <c r="F74" s="86" t="s">
         <v>1050</v>
-      </c>
-      <c r="F74" s="86" t="s">
-        <v>1051</v>
       </c>
       <c r="G74" s="86">
         <v>75000</v>
@@ -17943,22 +17940,22 @@
         <v>29</v>
       </c>
       <c r="C75" s="89" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D75" s="86" t="s">
+        <v>636</v>
+      </c>
+      <c r="E75" s="86" t="s">
+        <v>638</v>
+      </c>
+      <c r="F75" s="86" t="s">
         <v>637</v>
-      </c>
-      <c r="E75" s="86" t="s">
-        <v>639</v>
-      </c>
-      <c r="F75" s="86" t="s">
-        <v>638</v>
       </c>
       <c r="G75" s="86">
         <v>33549</v>
       </c>
       <c r="H75" s="86" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="76" spans="1:13">
@@ -17969,7 +17966,7 @@
         <v>29</v>
       </c>
       <c r="C76" s="89" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D76" s="86" t="s">
         <v>96</v>
@@ -17978,7 +17975,7 @@
         <v>556</v>
       </c>
       <c r="F76" s="86" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G76" s="86">
         <v>359539</v>
@@ -17990,10 +17987,10 @@
         <v>390</v>
       </c>
       <c r="J76" s="86" t="s">
+        <v>1054</v>
+      </c>
+      <c r="K76" s="86" t="s">
         <v>1055</v>
-      </c>
-      <c r="K76" s="86" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="77" spans="1:13">
@@ -18004,16 +18001,16 @@
         <v>29</v>
       </c>
       <c r="C77" s="89" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D77" s="86" t="s">
         <v>1057</v>
-      </c>
-      <c r="D77" s="86" t="s">
-        <v>1058</v>
       </c>
       <c r="E77" s="86" t="s">
         <v>185</v>
       </c>
       <c r="F77" s="86" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G77" s="86">
         <v>75000</v>
@@ -18033,22 +18030,22 @@
         <v>29</v>
       </c>
       <c r="C78" s="89" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D78" s="86" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E78" s="86" t="s">
         <v>492</v>
       </c>
       <c r="F78" s="86" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G78" s="86">
         <v>98275</v>
       </c>
       <c r="H78" s="86" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -18059,7 +18056,7 @@
         <v>29</v>
       </c>
       <c r="C79" s="89" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D79" s="86" t="s">
         <v>585</v>
@@ -18068,19 +18065,19 @@
         <v>347</v>
       </c>
       <c r="F79" s="86" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G79" s="86">
         <v>69997.67</v>
       </c>
       <c r="H79" s="86" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I79" s="86" t="s">
         <v>167</v>
       </c>
       <c r="J79" s="86" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>